<commit_message>
CU-1vc90uv api test for checking registering  of user
</commit_message>
<xml_diff>
--- a/qa/src/main/resources/ExcelRead.xlsx
+++ b/qa/src/main/resources/ExcelRead.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LoginTest" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="apiTest" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t xml:space="preserve">ValidUsername</t>
   </si>
@@ -83,6 +84,30 @@
   </si>
   <si>
     <t xml:space="preserve">Pass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">firstName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lastName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">srdjan.rados@htecgroup.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Qwertysha1@</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Srdjan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rados</t>
   </si>
 </sst>
 </file>
@@ -258,11 +283,11 @@
   </sheetPr>
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.01"/>
@@ -362,4 +387,65 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.42"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="srdjan.rados@htecgroup.com"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
CU-1vc90uv api test for checking registering  of user (#93)
* CU-1vc90uv api test for checking registering  of user

* CU-1vc90uv api test for checking registering  of user
</commit_message>
<xml_diff>
--- a/qa/src/main/resources/ExcelRead.xlsx
+++ b/qa/src/main/resources/ExcelRead.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LoginTest" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="apiTest" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t xml:space="preserve">ValidUsername</t>
   </si>
@@ -83,6 +84,30 @@
   </si>
   <si>
     <t xml:space="preserve">Pass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">firstName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lastName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">srdjan.rados@htecgroup.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Qwertysha1@</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Srdjan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rados</t>
   </si>
 </sst>
 </file>
@@ -258,11 +283,11 @@
   </sheetPr>
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.01"/>
@@ -362,4 +387,65 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.42"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="srdjan.rados@htecgroup.com"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
CU-1vhwepw added ntc for api Register
</commit_message>
<xml_diff>
--- a/qa/src/main/resources/ExcelRead.xlsx
+++ b/qa/src/main/resources/ExcelRead.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="30">
   <si>
     <t xml:space="preserve">ValidUsername</t>
   </si>
@@ -108,6 +108,9 @@
   </si>
   <si>
     <t xml:space="preserve">Rados</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Qwertysha</t>
   </si>
 </sst>
 </file>
@@ -287,7 +290,7 @@
       <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.01"/>
@@ -394,18 +397,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="36.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.41"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -436,9 +439,39 @@
         <v>28</v>
       </c>
     </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" display="srdjan.rados@htecgroup.com"/>
+    <hyperlink ref="A3" r:id="rId2" display="srdjan.rados@htecgroup"/>
+    <hyperlink ref="A4" r:id="rId3" display="srdjan.rados@htecgroup.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
CU-1vhwepw added ntc for api Register (#103)
* CU-1vhwepw added ntc for api Register

* CU-1vhwepw added ntc for api Register
</commit_message>
<xml_diff>
--- a/qa/src/main/resources/ExcelRead.xlsx
+++ b/qa/src/main/resources/ExcelRead.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
   <si>
     <t xml:space="preserve">ValidUsername</t>
   </si>
@@ -108,6 +108,12 @@
   </si>
   <si>
     <t xml:space="preserve">Rados</t>
+  </si>
+  <si>
+    <t xml:space="preserve">srdjan.rados@htecgroup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Qwertysha</t>
   </si>
 </sst>
 </file>
@@ -287,7 +293,7 @@
       <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.01"/>
@@ -394,18 +400,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="36.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.4"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -436,9 +442,39 @@
         <v>28</v>
       </c>
     </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" display="srdjan.rados@htecgroup.com"/>
+    <hyperlink ref="A3" r:id="rId2" display="srdjan.rados@htecgroup"/>
+    <hyperlink ref="A4" r:id="rId3" display="srdjan.rados@htecgroup.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
CU-1v6g3kh add changes to login page
</commit_message>
<xml_diff>
--- a/qa/src/main/resources/ExcelRead.xlsx
+++ b/qa/src/main/resources/ExcelRead.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="LoginTest" sheetId="1" state="visible" r:id="rId2"/>
@@ -120,8 +120,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -200,12 +201,16 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -289,11 +294,11 @@
   </sheetPr>
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.01"/>
@@ -370,6 +375,7 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C5" s="2"/>
       <c r="D5" s="0" t="s">
         <v>19</v>
       </c>
@@ -402,11 +408,11 @@
   </sheetPr>
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="36.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.61"/>

</xml_diff>

<commit_message>
CU-1wm69wb update user by id
</commit_message>
<xml_diff>
--- a/qa/src/main/resources/ExcelRead.xlsx
+++ b/qa/src/main/resources/ExcelRead.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
   <si>
     <t xml:space="preserve">ValidUsername</t>
   </si>
@@ -98,6 +98,15 @@
     <t xml:space="preserve">lastName</t>
   </si>
   <si>
+    <t xml:space="preserve">New-firstName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New-lastName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New-pass</t>
+  </si>
+  <si>
     <t xml:space="preserve">srdjan.rados@htecgroup.com</t>
   </si>
   <si>
@@ -108,6 +117,15 @@
   </si>
   <si>
     <t xml:space="preserve">Rados</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Srdjan1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rados1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test123@</t>
   </si>
   <si>
     <t xml:space="preserve">srdjan.rados@htecgroup</t>
@@ -293,7 +311,7 @@
       <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.01"/>
@@ -400,21 +418,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="36.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="20.14"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>21</v>
       </c>
@@ -427,47 +448,65 @@
       <c r="D1" s="0" t="s">
         <v>24</v>
       </c>
+      <c r="E1" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>26</v>
-      </c>
       <c r="C3" s="0" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B4" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="0" t="s">
-        <v>27</v>
-      </c>
       <c r="D4" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added test suit and test runner (#145)
* CU-1v6g3kh add changes to login page

* CU-1v6g3kh added_changes_on_login_page

* CU-1wm4gyw implemented_test_suit_class

* Delete TestRunner.java
</commit_message>
<xml_diff>
--- a/qa/src/main/resources/ExcelRead.xlsx
+++ b/qa/src/main/resources/ExcelRead.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="LoginTest" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
   <si>
     <t xml:space="preserve">ValidUsername</t>
   </si>
@@ -44,13 +44,13 @@
     <t xml:space="preserve">SuccessfulText</t>
   </si>
   <si>
-    <t xml:space="preserve">peraperic@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Password.123</t>
-  </si>
-  <si>
-    <t xml:space="preserve">perapericgmail.com</t>
+    <t xml:space="preserve">lidija.veljkovic@htecgroup.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lazanja29#</t>
+  </si>
+  <si>
+    <t xml:space="preserve">peraperic@gmailcom</t>
   </si>
   <si>
     <t xml:space="preserve">password.123</t>
@@ -62,19 +62,10 @@
     <t xml:space="preserve">pera.peric@gmail.com</t>
   </si>
   <si>
-    <t xml:space="preserve">peraperic@gmailcom</t>
-  </si>
-  <si>
     <t xml:space="preserve">PASSWORD.123</t>
   </si>
   <si>
     <t xml:space="preserve">Sign Up</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pera1@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">peraperic@gmail</t>
   </si>
   <si>
     <t xml:space="preserve">Password#</t>
@@ -120,10 +111,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -153,6 +145,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -200,12 +198,24 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -289,13 +299,13 @@
   </sheetPr>
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.76953125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.29"/>
@@ -334,7 +344,7 @@
       <c r="B2" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D2" s="0" t="s">
@@ -348,42 +358,39 @@
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="B3" s="3"/>
       <c r="C3" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="E3" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="0" t="s">
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4"/>
+      <c r="D4" s="0" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C5" s="3"/>
+      <c r="D5" s="0" t="s">
         <v>16</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D5" s="0" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D6" s="0" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="peraperic@gmail.com"/>
-    <hyperlink ref="A3" r:id="rId2" display="pera.peric@gmail.com"/>
-    <hyperlink ref="A4" r:id="rId3" display="pera1@gmail.com"/>
+    <hyperlink ref="A2" r:id="rId1" display="lidija.veljkovic@htecgroup.com"/>
+    <hyperlink ref="C2" r:id="rId2" display="peraperic@gmailcom"/>
+    <hyperlink ref="A3" r:id="rId3" display="pera.peric@gmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -402,11 +409,11 @@
   </sheetPr>
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="36.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.61"/>
@@ -416,58 +423,58 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="0" t="s">
         <v>21</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="0" t="s">
         <v>25</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="0" t="s">
         <v>25</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
CU-1wu0tud refactoring apiTest with RestFunctionHelpers
</commit_message>
<xml_diff>
--- a/qa/src/main/resources/ExcelRead.xlsx
+++ b/qa/src/main/resources/ExcelRead.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LoginTest" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="34">
   <si>
     <t xml:space="preserve">ValidUsername</t>
   </si>
@@ -89,6 +89,15 @@
     <t xml:space="preserve">lastName</t>
   </si>
   <si>
+    <t xml:space="preserve">newFirstName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newLastName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newPass</t>
+  </si>
+  <si>
     <t xml:space="preserve">srdjan.rados@htecgroup.com</t>
   </si>
   <si>
@@ -99,6 +108,15 @@
   </si>
   <si>
     <t xml:space="preserve">Rados</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Srdjan1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rados1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test123@</t>
   </si>
   <si>
     <t xml:space="preserve">srdjan.rados@htecgroup</t>
@@ -115,7 +133,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -146,12 +164,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -207,7 +219,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -299,11 +311,11 @@
   </sheetPr>
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.76953125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.78515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.01"/>
@@ -407,21 +419,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="36.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="21.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.81"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>18</v>
       </c>
@@ -434,47 +449,65 @@
       <c r="D1" s="0" t="s">
         <v>21</v>
       </c>
+      <c r="E1" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>23</v>
-      </c>
       <c r="C3" s="0" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B4" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="0" t="s">
-        <v>24</v>
-      </c>
       <c r="D4" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
CU-1wu0tud refactoring apiTest with RestFunctionHelpers (#148)
</commit_message>
<xml_diff>
--- a/qa/src/main/resources/ExcelRead.xlsx
+++ b/qa/src/main/resources/ExcelRead.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LoginTest" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="34">
   <si>
     <t xml:space="preserve">ValidUsername</t>
   </si>
@@ -89,6 +89,15 @@
     <t xml:space="preserve">lastName</t>
   </si>
   <si>
+    <t xml:space="preserve">newFirstName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newLastName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newPass</t>
+  </si>
+  <si>
     <t xml:space="preserve">srdjan.rados@htecgroup.com</t>
   </si>
   <si>
@@ -99,6 +108,15 @@
   </si>
   <si>
     <t xml:space="preserve">Rados</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Srdjan1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rados1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test123@</t>
   </si>
   <si>
     <t xml:space="preserve">srdjan.rados@htecgroup</t>
@@ -115,7 +133,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -146,12 +164,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -207,7 +219,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -299,11 +311,11 @@
   </sheetPr>
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.76953125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.78515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.01"/>
@@ -407,21 +419,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="36.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="21.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.81"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>18</v>
       </c>
@@ -434,47 +449,65 @@
       <c r="D1" s="0" t="s">
         <v>21</v>
       </c>
+      <c r="E1" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>23</v>
-      </c>
       <c r="C3" s="0" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B4" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="0" t="s">
-        <v>24</v>
-      </c>
       <c r="D4" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "CU-1wu0tud refactoring apiTest with RestFunctionHelpers (#148)"
This reverts commit 7495d676b5f978a38ac344ce14dcacbd5a39a0c3.
</commit_message>
<xml_diff>
--- a/qa/src/main/resources/ExcelRead.xlsx
+++ b/qa/src/main/resources/ExcelRead.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="LoginTest" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
   <si>
     <t xml:space="preserve">ValidUsername</t>
   </si>
@@ -89,15 +89,6 @@
     <t xml:space="preserve">lastName</t>
   </si>
   <si>
-    <t xml:space="preserve">newFirstName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">newLastName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">newPass</t>
-  </si>
-  <si>
     <t xml:space="preserve">srdjan.rados@htecgroup.com</t>
   </si>
   <si>
@@ -108,15 +99,6 @@
   </si>
   <si>
     <t xml:space="preserve">Rados</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Srdjan1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rados1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test123@</t>
   </si>
   <si>
     <t xml:space="preserve">srdjan.rados@htecgroup</t>
@@ -133,7 +115,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -163,6 +145,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -219,7 +207,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -311,11 +299,11 @@
   </sheetPr>
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.78515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.76953125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.01"/>
@@ -419,24 +407,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="36.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="21.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.4"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>18</v>
       </c>
@@ -449,65 +434,47 @@
       <c r="D1" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="F1" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="G1" s="0" t="s">
-        <v>24</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="0" t="s">
         <v>25</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="G2" s="0" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="0" t="s">
         <v>25</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "CU-1wu0tud refactoring apiTest with RestFunctionHelpers (#148)" (#155)
This reverts commit 7495d676b5f978a38ac344ce14dcacbd5a39a0c3.
</commit_message>
<xml_diff>
--- a/qa/src/main/resources/ExcelRead.xlsx
+++ b/qa/src/main/resources/ExcelRead.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="LoginTest" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
   <si>
     <t xml:space="preserve">ValidUsername</t>
   </si>
@@ -89,15 +89,6 @@
     <t xml:space="preserve">lastName</t>
   </si>
   <si>
-    <t xml:space="preserve">newFirstName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">newLastName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">newPass</t>
-  </si>
-  <si>
     <t xml:space="preserve">srdjan.rados@htecgroup.com</t>
   </si>
   <si>
@@ -108,15 +99,6 @@
   </si>
   <si>
     <t xml:space="preserve">Rados</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Srdjan1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rados1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test123@</t>
   </si>
   <si>
     <t xml:space="preserve">srdjan.rados@htecgroup</t>
@@ -133,7 +115,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -163,6 +145,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -219,7 +207,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -311,11 +299,11 @@
   </sheetPr>
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.78515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.76953125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.01"/>
@@ -419,24 +407,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="36.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="21.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.4"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>18</v>
       </c>
@@ -449,65 +434,47 @@
       <c r="D1" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="F1" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="G1" s="0" t="s">
-        <v>24</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="0" t="s">
         <v>25</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="G2" s="0" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="0" t="s">
         <v>25</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
CU-1wu0tud code refactoring after reverting
</commit_message>
<xml_diff>
--- a/qa/src/main/resources/ExcelRead.xlsx
+++ b/qa/src/main/resources/ExcelRead.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LoginTest" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="apiTest" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="RegistrationTest" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="55">
   <si>
     <t xml:space="preserve">ValidUsername</t>
   </si>
@@ -44,30 +45,39 @@
     <t xml:space="preserve">SuccessfulText</t>
   </si>
   <si>
-    <t xml:space="preserve">lidija.veljkovic@htecgroup.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lazanja29#</t>
+    <t xml:space="preserve">peraperic@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Password.123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">perapericgmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">password.123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sign In</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pera.peric@gmail.com</t>
   </si>
   <si>
     <t xml:space="preserve">peraperic@gmailcom</t>
   </si>
   <si>
-    <t xml:space="preserve">password.123</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sign In</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pera.peric@gmail.com</t>
-  </si>
-  <si>
     <t xml:space="preserve">PASSWORD.123</t>
   </si>
   <si>
     <t xml:space="preserve">Sign Up</t>
   </si>
   <si>
+    <t xml:space="preserve">pera1@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">peraperic@gmail</t>
+  </si>
+  <si>
     <t xml:space="preserve">Password#</t>
   </si>
   <si>
@@ -89,6 +99,15 @@
     <t xml:space="preserve">lastName</t>
   </si>
   <si>
+    <t xml:space="preserve">New-firstName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New-lastName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New-pass</t>
+  </si>
+  <si>
     <t xml:space="preserve">srdjan.rados@htecgroup.com</t>
   </si>
   <si>
@@ -101,10 +120,73 @@
     <t xml:space="preserve">Rados</t>
   </si>
   <si>
+    <t xml:space="preserve">Srdjan1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rados1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test123@</t>
+  </si>
+  <si>
     <t xml:space="preserve">srdjan.rados@htecgroup</t>
   </si>
   <si>
     <t xml:space="preserve">Qwertysha</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ValidEmail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ValidFirstName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ValidLastName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">InvalidEmail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">InvalidPassword</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stefanzgajic@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shelf1@7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stefan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gajic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stefanzgajicgmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shelf!@7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stefanzgajic@gmailcom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shelf!@k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stefanzgajic@@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SHELF1@7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stefanzgajic@gmail..com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shelf107</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shelf!@</t>
   </si>
 </sst>
 </file>
@@ -115,7 +197,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -146,12 +228,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -198,7 +274,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -207,15 +283,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -299,13 +367,13 @@
   </sheetPr>
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.76953125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.82421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.29"/>
@@ -344,7 +412,7 @@
       <c r="B2" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="0" t="s">
         <v>9</v>
       </c>
       <c r="D2" s="0" t="s">
@@ -358,39 +426,42 @@
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="3"/>
       <c r="C3" s="0" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4"/>
+      <c r="A4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>17</v>
+      </c>
       <c r="D4" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C5" s="3"/>
       <c r="D5" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D6" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="lidija.veljkovic@htecgroup.com"/>
-    <hyperlink ref="C2" r:id="rId2" display="peraperic@gmailcom"/>
-    <hyperlink ref="A3" r:id="rId3" display="pera.peric@gmail.com"/>
+    <hyperlink ref="A2" r:id="rId1" display="peraperic@gmail.com"/>
+    <hyperlink ref="A3" r:id="rId2" display="pera.peric@gmail.com"/>
+    <hyperlink ref="A4" r:id="rId3" display="pera1@gmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -407,74 +478,94 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="36.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.08"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>21</v>
+        <v>24</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>25</v>
+        <v>31</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -484,11 +575,137 @@
     <hyperlink ref="A4" r:id="rId3" display="srdjan.rados@htecgroup.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageMargins left="0.7875" right="0.7875" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E19" activeCellId="0" sqref="E19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="13.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="23.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.18"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="stefanzgajic@gmail.com"/>
+    <hyperlink ref="B2" r:id="rId2" display="Shelf1@7"/>
+    <hyperlink ref="F2" r:id="rId3" display="shelf!@7"/>
+    <hyperlink ref="E3" r:id="rId4" display="stefanzgajic@gmailcom"/>
+    <hyperlink ref="F3" r:id="rId5" display="Shelf!@k"/>
+    <hyperlink ref="F4" r:id="rId6" display="SHELF1@7"/>
+    <hyperlink ref="E5" r:id="rId7" display="stefanzgajic@gmail..com"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
CU-1wu0tud code refactoring after reverting (#160)
</commit_message>
<xml_diff>
--- a/qa/src/main/resources/ExcelRead.xlsx
+++ b/qa/src/main/resources/ExcelRead.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LoginTest" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="apiTest" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="RegistrationTest" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="55">
   <si>
     <t xml:space="preserve">ValidUsername</t>
   </si>
@@ -44,30 +45,39 @@
     <t xml:space="preserve">SuccessfulText</t>
   </si>
   <si>
-    <t xml:space="preserve">lidija.veljkovic@htecgroup.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lazanja29#</t>
+    <t xml:space="preserve">peraperic@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Password.123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">perapericgmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">password.123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sign In</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pera.peric@gmail.com</t>
   </si>
   <si>
     <t xml:space="preserve">peraperic@gmailcom</t>
   </si>
   <si>
-    <t xml:space="preserve">password.123</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sign In</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pera.peric@gmail.com</t>
-  </si>
-  <si>
     <t xml:space="preserve">PASSWORD.123</t>
   </si>
   <si>
     <t xml:space="preserve">Sign Up</t>
   </si>
   <si>
+    <t xml:space="preserve">pera1@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">peraperic@gmail</t>
+  </si>
+  <si>
     <t xml:space="preserve">Password#</t>
   </si>
   <si>
@@ -89,6 +99,15 @@
     <t xml:space="preserve">lastName</t>
   </si>
   <si>
+    <t xml:space="preserve">New-firstName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New-lastName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New-pass</t>
+  </si>
+  <si>
     <t xml:space="preserve">srdjan.rados@htecgroup.com</t>
   </si>
   <si>
@@ -101,10 +120,73 @@
     <t xml:space="preserve">Rados</t>
   </si>
   <si>
+    <t xml:space="preserve">Srdjan1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rados1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test123@</t>
+  </si>
+  <si>
     <t xml:space="preserve">srdjan.rados@htecgroup</t>
   </si>
   <si>
     <t xml:space="preserve">Qwertysha</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ValidEmail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ValidFirstName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ValidLastName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">InvalidEmail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">InvalidPassword</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stefanzgajic@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shelf1@7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stefan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gajic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stefanzgajicgmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shelf!@7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stefanzgajic@gmailcom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shelf!@k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stefanzgajic@@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SHELF1@7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stefanzgajic@gmail..com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shelf107</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shelf!@</t>
   </si>
 </sst>
 </file>
@@ -115,7 +197,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -146,12 +228,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -198,7 +274,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -207,15 +283,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -299,13 +367,13 @@
   </sheetPr>
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.76953125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.82421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.29"/>
@@ -344,7 +412,7 @@
       <c r="B2" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="0" t="s">
         <v>9</v>
       </c>
       <c r="D2" s="0" t="s">
@@ -358,39 +426,42 @@
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="3"/>
       <c r="C3" s="0" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4"/>
+      <c r="A4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>17</v>
+      </c>
       <c r="D4" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C5" s="3"/>
       <c r="D5" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D6" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="lidija.veljkovic@htecgroup.com"/>
-    <hyperlink ref="C2" r:id="rId2" display="peraperic@gmailcom"/>
-    <hyperlink ref="A3" r:id="rId3" display="pera.peric@gmail.com"/>
+    <hyperlink ref="A2" r:id="rId1" display="peraperic@gmail.com"/>
+    <hyperlink ref="A3" r:id="rId2" display="pera.peric@gmail.com"/>
+    <hyperlink ref="A4" r:id="rId3" display="pera1@gmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -407,74 +478,94 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="36.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.08"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>21</v>
+        <v>24</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>25</v>
+        <v>31</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -484,11 +575,137 @@
     <hyperlink ref="A4" r:id="rId3" display="srdjan.rados@htecgroup.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageMargins left="0.7875" right="0.7875" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E19" activeCellId="0" sqref="E19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="13.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="23.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.18"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="stefanzgajic@gmail.com"/>
+    <hyperlink ref="B2" r:id="rId2" display="Shelf1@7"/>
+    <hyperlink ref="F2" r:id="rId3" display="shelf!@7"/>
+    <hyperlink ref="E3" r:id="rId4" display="stefanzgajic@gmailcom"/>
+    <hyperlink ref="F3" r:id="rId5" display="Shelf!@k"/>
+    <hyperlink ref="F4" r:id="rId6" display="SHELF1@7"/>
+    <hyperlink ref="E5" r:id="rId7" display="stefanzgajic@gmail..com"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
CU-1yrwt71 added UI tests for registration and code refactoring
</commit_message>
<xml_diff>
--- a/qa/src/main/resources/ExcelRead.xlsx
+++ b/qa/src/main/resources/ExcelRead.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="LoginTest" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="57">
   <si>
     <t xml:space="preserve">ValidUsername</t>
   </si>
@@ -138,6 +138,12 @@
     <t xml:space="preserve">InvalidPassword</t>
   </si>
   <si>
+    <t xml:space="preserve">InvalidFirstName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">InvalidLastName</t>
+  </si>
+  <si>
     <t xml:space="preserve">stefanzgajic@gmail.com</t>
   </si>
   <si>
@@ -156,6 +162,12 @@
     <t xml:space="preserve">shelf!@7</t>
   </si>
   <si>
+    <t xml:space="preserve">StefanStefanStefanStefanStefanStefanStefanStefanSte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GajicGajicGajicGajicGajicGajicGajicGajicGajicGajicG</t>
+  </si>
+  <si>
     <t xml:space="preserve">stefanzgajic@gmailcom</t>
   </si>
   <si>
@@ -174,7 +186,13 @@
     <t xml:space="preserve">Shelf107</t>
   </si>
   <si>
+    <t xml:space="preserve">stefan.zgajic.stefan.zgajic.stefan.zgajic@gmail.com</t>
+  </si>
+  <si>
     <t xml:space="preserve">Shelf!@</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shelf!@7Shelf!@7Shelf!@7Shelf!@7Shelf!@7Shelf!@7!@7</t>
   </si>
 </sst>
 </file>
@@ -359,11 +377,11 @@
   </sheetPr>
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84765625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.01"/>
@@ -471,7 +489,7 @@
       <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.65"/>
@@ -576,19 +594,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E19" activeCellId="0" sqref="E19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F9" activeCellId="0" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="13.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="23.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="43.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="51.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="46.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="43.12"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -610,25 +630,37 @@
       <c r="F1" s="3" t="s">
         <v>37</v>
       </c>
+      <c r="G1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>43</v>
+        <v>45</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -637,11 +669,13 @@
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>45</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="G3" s="2"/>
+      <c r="H3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3"/>
@@ -649,11 +683,13 @@
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>47</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3"/>
@@ -661,32 +697,51 @@
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>49</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
+      <c r="E6" s="3" t="s">
+        <v>54</v>
+      </c>
       <c r="F6" s="3" t="s">
-        <v>50</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="stefanzgajic@gmail.com"/>
-    <hyperlink ref="B2" r:id="rId2" display="Shelf1@7"/>
-    <hyperlink ref="F2" r:id="rId3" display="shelf!@7"/>
-    <hyperlink ref="E3" r:id="rId4" display="stefanzgajic@gmailcom"/>
-    <hyperlink ref="F3" r:id="rId5" display="Shelf!@k"/>
-    <hyperlink ref="F4" r:id="rId6" display="SHELF1@7"/>
-    <hyperlink ref="E5" r:id="rId7" display="stefanzgajic@gmail..com"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
CU-1yrwt71 added UI tests for registration and code refactoring (#263)
</commit_message>
<xml_diff>
--- a/qa/src/main/resources/ExcelRead.xlsx
+++ b/qa/src/main/resources/ExcelRead.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="LoginTest" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="57">
   <si>
     <t xml:space="preserve">ValidUsername</t>
   </si>
@@ -138,6 +138,12 @@
     <t xml:space="preserve">InvalidPassword</t>
   </si>
   <si>
+    <t xml:space="preserve">InvalidFirstName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">InvalidLastName</t>
+  </si>
+  <si>
     <t xml:space="preserve">stefanzgajic@gmail.com</t>
   </si>
   <si>
@@ -156,6 +162,12 @@
     <t xml:space="preserve">shelf!@7</t>
   </si>
   <si>
+    <t xml:space="preserve">StefanStefanStefanStefanStefanStefanStefanStefanSte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GajicGajicGajicGajicGajicGajicGajicGajicGajicGajicG</t>
+  </si>
+  <si>
     <t xml:space="preserve">stefanzgajic@gmailcom</t>
   </si>
   <si>
@@ -174,7 +186,13 @@
     <t xml:space="preserve">Shelf107</t>
   </si>
   <si>
+    <t xml:space="preserve">stefan.zgajic.stefan.zgajic.stefan.zgajic@gmail.com</t>
+  </si>
+  <si>
     <t xml:space="preserve">Shelf!@</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shelf!@7Shelf!@7Shelf!@7Shelf!@7Shelf!@7Shelf!@7!@7</t>
   </si>
 </sst>
 </file>
@@ -359,11 +377,11 @@
   </sheetPr>
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84765625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.01"/>
@@ -471,7 +489,7 @@
       <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.65"/>
@@ -576,19 +594,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E19" activeCellId="0" sqref="E19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F9" activeCellId="0" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="13.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="23.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="43.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="51.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="46.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="43.12"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -610,25 +630,37 @@
       <c r="F1" s="3" t="s">
         <v>37</v>
       </c>
+      <c r="G1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>43</v>
+        <v>45</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -637,11 +669,13 @@
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>45</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="G3" s="2"/>
+      <c r="H3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3"/>
@@ -649,11 +683,13 @@
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>47</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3"/>
@@ -661,32 +697,51 @@
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>49</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
+      <c r="E6" s="3" t="s">
+        <v>54</v>
+      </c>
       <c r="F6" s="3" t="s">
-        <v>50</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="stefanzgajic@gmail.com"/>
-    <hyperlink ref="B2" r:id="rId2" display="Shelf1@7"/>
-    <hyperlink ref="F2" r:id="rId3" display="shelf!@7"/>
-    <hyperlink ref="E3" r:id="rId4" display="stefanzgajic@gmailcom"/>
-    <hyperlink ref="F3" r:id="rId5" display="Shelf!@k"/>
-    <hyperlink ref="F4" r:id="rId6" display="SHELF1@7"/>
-    <hyperlink ref="E5" r:id="rId7" display="stefanzgajic@gmail..com"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="0.7875" bottom="0.7875" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>